<commit_message>
Started work with the deal and firm charactersitics
Sensitivity analysis
</commit_message>
<xml_diff>
--- a/data/final/model1_trim_used_data.xlsx
+++ b/data/final/model1_trim_used_data.xlsx
@@ -1909,7 +1909,7 @@
         <v>0.7849668810598061</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2209,7 +2209,7 @@
         <v>2.659773510585918</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2259,7 +2259,7 @@
         <v>-49.72222222222222</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2759,7 +2759,7 @@
         <v>3.441941581546289</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -2809,7 +2809,7 @@
         <v>5.488939172385821</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2859,7 +2859,7 @@
         <v>2.173709810103347</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -2909,7 +2909,7 @@
         <v>2.292970362678743</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>0.75</v>
@@ -2959,7 +2959,7 @@
         <v>3.514946034953418</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3059,7 +3059,7 @@
         <v>0.6722777485533928</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3109,7 +3109,7 @@
         <v>8.664201183431953</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3159,7 +3159,7 @@
         <v>2.77012158476261</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3209,7 +3209,7 @@
         <v>2.049264254161425</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0.6</v>
@@ -3309,7 +3309,7 @@
         <v>2.576147130599215</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>8.35587987650856</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3409,7 +3409,7 @@
         <v>20.85430463576159</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3459,7 +3459,7 @@
         <v>3.990717821782178</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4159,7 +4159,7 @@
         <v>8.029020433325956</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>0.5</v>
@@ -4209,7 +4209,7 @@
         <v>1.294709973496505</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>0.5</v>
@@ -6009,7 +6009,7 @@
         <v>0.7262594739188586</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -6159,7 +6159,7 @@
         <v>5.500690607734807</v>
       </c>
       <c r="G116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -6209,7 +6209,7 @@
         <v>3.969798533539857</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -6259,7 +6259,7 @@
         <v>1.974688699857873</v>
       </c>
       <c r="G118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H118">
         <v>0.5714285714285714</v>
@@ -6309,7 +6309,7 @@
         <v>8.932279133722929</v>
       </c>
       <c r="G119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H119">
         <v>0.4</v>
@@ -6359,7 +6359,7 @@
         <v>4.524524472280214</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -6409,7 +6409,7 @@
         <v>5.621591174782663</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H121">
         <v>0</v>
@@ -6459,7 +6459,7 @@
         <v>2.1746402952475</v>
       </c>
       <c r="G122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H122">
         <v>0.3333333333333333</v>
@@ -6509,7 +6509,7 @@
         <v>1.55502235794525</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -6559,7 +6559,7 @@
         <v>6.15708288482239</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -9059,7 +9059,7 @@
         <v>3.881906161950264</v>
       </c>
       <c r="G174">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H174">
         <v>1</v>
@@ -9359,7 +9359,7 @@
         <v>23.21992590500557</v>
       </c>
       <c r="G180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H180">
         <v>0</v>
@@ -9409,7 +9409,7 @@
         <v>6.994072865687873</v>
       </c>
       <c r="G181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H181">
         <v>0.6666666666666666</v>
@@ -9459,7 +9459,7 @@
         <v>1.952416356877324</v>
       </c>
       <c r="G182">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H182">
         <v>0</v>
@@ -9509,7 +9509,7 @@
         <v>11.64652825051055</v>
       </c>
       <c r="G183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H183">
         <v>0</v>
@@ -9559,7 +9559,7 @@
         <v>6.465940054495913</v>
       </c>
       <c r="G184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -9609,7 +9609,7 @@
         <v>1.140045805411825</v>
       </c>
       <c r="G185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H185">
         <v>0</v>
@@ -9659,7 +9659,7 @@
         <v>2.432248196868708</v>
       </c>
       <c r="G186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H186">
         <v>0.4285714285714285</v>
@@ -9709,7 +9709,7 @@
         <v>4.053581191908147</v>
       </c>
       <c r="G187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H187">
         <v>0</v>
@@ -11459,7 +11459,7 @@
         <v>1.533681214421252</v>
       </c>
       <c r="G222">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H222">
         <v>0</v>
@@ -11509,7 +11509,7 @@
         <v>2.922535211267606</v>
       </c>
       <c r="G223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H223">
         <v>0</v>
@@ -11559,7 +11559,7 @@
         <v>5.243420796890184</v>
       </c>
       <c r="G224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H224">
         <v>0.2</v>
@@ -11609,7 +11609,7 @@
         <v>2.538361508452536</v>
       </c>
       <c r="G225">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H225">
         <v>0</v>
@@ -11659,7 +11659,7 @@
         <v>0.835633728268393</v>
       </c>
       <c r="G226">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H226">
         <v>0.5</v>
@@ -11709,7 +11709,7 @@
         <v>3.397668453117127</v>
       </c>
       <c r="G227">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H227">
         <v>0.5555555555555556</v>
@@ -11759,7 +11759,7 @@
         <v>4.121447411314939</v>
       </c>
       <c r="G228">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H228">
         <v>0</v>
@@ -11809,7 +11809,7 @@
         <v>14.70716009654063</v>
       </c>
       <c r="G229">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H229">
         <v>0</v>
@@ -11859,7 +11859,7 @@
         <v>1.276943193374982</v>
       </c>
       <c r="G230">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H230">
         <v>0</v>
@@ -11909,7 +11909,7 @@
         <v>5.363262237347156</v>
       </c>
       <c r="G231">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H231">
         <v>0.3333333333333333</v>
@@ -11959,7 +11959,7 @@
         <v>3.200833397904452</v>
       </c>
       <c r="G232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -12009,7 +12009,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="G233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H233">
         <v>0</v>
@@ -12059,7 +12059,7 @@
         <v>5.115170327921044</v>
       </c>
       <c r="G234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H234">
         <v>0</v>
@@ -12109,7 +12109,7 @@
         <v>16.32722398245187</v>
       </c>
       <c r="G235">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H235">
         <v>0.4</v>
@@ -12159,7 +12159,7 @@
         <v>1.42512077294686</v>
       </c>
       <c r="G236">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H236">
         <v>0</v>
@@ -12209,7 +12209,7 @@
         <v>3.118185239192813</v>
       </c>
       <c r="G237">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H237">
         <v>0.6</v>
@@ -12259,7 +12259,7 @@
         <v>1.758633324173308</v>
       </c>
       <c r="G238">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H238">
         <v>0</v>
@@ -12309,7 +12309,7 @@
         <v>3.543876689189189</v>
       </c>
       <c r="G239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H239">
         <v>0</v>
@@ -12359,7 +12359,7 @@
         <v>168.5253456221198</v>
       </c>
       <c r="G240">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H240">
         <v>0</v>
@@ -12409,7 +12409,7 @@
         <v>6.39110686110447</v>
       </c>
       <c r="G241">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H241">
         <v>0</v>
@@ -12459,7 +12459,7 @@
         <v>0.7595595568245468</v>
       </c>
       <c r="G242">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H242">
         <v>0</v>
@@ -12509,7 +12509,7 @@
         <v>3.684466019417476</v>
       </c>
       <c r="G243">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H243">
         <v>0</v>
@@ -12559,7 +12559,7 @@
         <v>2.85305889079474</v>
       </c>
       <c r="G244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -12609,7 +12609,7 @@
         <v>3.379772510340439</v>
       </c>
       <c r="G245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H245">
         <v>0</v>

</xml_diff>